<commit_message>
Changed header color to gray
</commit_message>
<xml_diff>
--- a/GradeBook_Unsolved bc.xlsx
+++ b/GradeBook_Unsolved bc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrobertciminera/Library/Mobile Documents/com~apple~CloudDocs/Columbia Data Analytics and Visualization /1-Student-Resources/02-Stu_GradeBook/Unsolved/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3A2BD43-3164-B746-ABB1-226BBC66E24B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD3D385-6C3C-6043-9803-FE6DCB19827F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27960" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="320" yWindow="2240" windowWidth="27960" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -222,12 +222,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -255,9 +261,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -268,6 +271,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -587,7 +593,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -598,28 +604,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -627,57 +633,57 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>85</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>84</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>90</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>56</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <f>ROUND(AVERAGE(B2:E2),0)</f>
         <v>79</v>
       </c>
-      <c r="G2" s="2" t="str">
+      <c r="G2" s="1" t="str">
         <f>IF(F2&lt;=60,"Fail","Pass")</f>
         <v>Pass</v>
       </c>
-      <c r="H2" s="2" t="str">
+      <c r="H2" s="1" t="str">
         <f>IF(F2&gt;89,"A",IF(F2&gt;79,"B",IF(F2&gt;69,"C",IF(F2&gt;59,"D","F"))))</f>
         <v>C</v>
       </c>
-      <c r="I2" s="5"/>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>48</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>57</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>97</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>95</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <f t="shared" ref="F3:F25" si="0">ROUND(AVERAGE(B3:E3),0)</f>
         <v>74</v>
       </c>
-      <c r="G3" s="2" t="str">
+      <c r="G3" s="1" t="str">
         <f t="shared" ref="G3:G25" si="1">IF(F3&lt;=60,"Fail","Pass")</f>
         <v>Pass</v>
       </c>
-      <c r="H3" s="2" t="str">
+      <c r="H3" s="1" t="str">
         <f t="shared" ref="H3:H25" si="2">IF(F3&gt;89,"A",IF(F3&gt;79,"B",IF(F3&gt;69,"C",IF(F3&gt;59,"D","F"))))</f>
         <v>C</v>
       </c>
@@ -686,27 +692,27 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>96</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>100</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>97</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>87</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
-      <c r="G4" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>Pass</v>
-      </c>
-      <c r="H4" s="2" t="str">
+      <c r="G4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Pass</v>
+      </c>
+      <c r="H4" s="1" t="str">
         <f t="shared" si="2"/>
         <v>A</v>
       </c>
@@ -715,27 +721,27 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>52</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>52</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>64</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>63</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="G5" s="2" t="str">
+      <c r="G5" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Fail</v>
       </c>
-      <c r="H5" s="2" t="str">
+      <c r="H5" s="1" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -744,27 +750,27 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>89</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>57</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>90</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>85</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="G6" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>Pass</v>
-      </c>
-      <c r="H6" s="2" t="str">
+      <c r="G6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Pass</v>
+      </c>
+      <c r="H6" s="1" t="str">
         <f t="shared" si="2"/>
         <v>B</v>
       </c>
@@ -773,27 +779,27 @@
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>71</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>93</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>97</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>55</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
-      <c r="G7" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>Pass</v>
-      </c>
-      <c r="H7" s="2" t="str">
+      <c r="G7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Pass</v>
+      </c>
+      <c r="H7" s="1" t="str">
         <f t="shared" si="2"/>
         <v>C</v>
       </c>
@@ -802,27 +808,27 @@
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>97</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>90</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>70</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>83</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="G8" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>Pass</v>
-      </c>
-      <c r="H8" s="2" t="str">
+      <c r="G8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Pass</v>
+      </c>
+      <c r="H8" s="1" t="str">
         <f t="shared" si="2"/>
         <v>B</v>
       </c>
@@ -831,27 +837,27 @@
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>67</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>62</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>48</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>43</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="G9" s="2" t="str">
+      <c r="G9" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Fail</v>
       </c>
-      <c r="H9" s="2" t="str">
+      <c r="H9" s="1" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -860,27 +866,27 @@
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>100</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>94</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>90</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>95</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
-      <c r="G10" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>Pass</v>
-      </c>
-      <c r="H10" s="2" t="str">
+      <c r="G10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Pass</v>
+      </c>
+      <c r="H10" s="1" t="str">
         <f t="shared" si="2"/>
         <v>A</v>
       </c>
@@ -889,27 +895,27 @@
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>88</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>61</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>45</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>47</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="G11" s="2" t="str">
+      <c r="G11" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Fail</v>
       </c>
-      <c r="H11" s="2" t="str">
+      <c r="H11" s="1" t="str">
         <f t="shared" si="2"/>
         <v>D</v>
       </c>
@@ -918,27 +924,27 @@
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>44</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>87</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>43</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>55</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="G12" s="2" t="str">
+      <c r="G12" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Fail</v>
       </c>
-      <c r="H12" s="2" t="str">
+      <c r="H12" s="1" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -947,27 +953,27 @@
       <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>83</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>42</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>67</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>46</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="G13" s="2" t="str">
+      <c r="G13" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Fail</v>
       </c>
-      <c r="H13" s="2" t="str">
+      <c r="H13" s="1" t="str">
         <f t="shared" si="2"/>
         <v>D</v>
       </c>
@@ -976,27 +982,27 @@
       <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>59</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>43</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>43</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>52</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="G14" s="2" t="str">
+      <c r="G14" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Fail</v>
       </c>
-      <c r="H14" s="2" t="str">
+      <c r="H14" s="1" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -1005,27 +1011,27 @@
       <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>54</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>47</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>92</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>57</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="G15" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>Pass</v>
-      </c>
-      <c r="H15" s="2" t="str">
+      <c r="G15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Pass</v>
+      </c>
+      <c r="H15" s="1" t="str">
         <f t="shared" si="2"/>
         <v>D</v>
       </c>
@@ -1034,27 +1040,27 @@
       <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>73</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>98</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>59</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>73</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
-      <c r="G16" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>Pass</v>
-      </c>
-      <c r="H16" s="2" t="str">
+      <c r="G16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Pass</v>
+      </c>
+      <c r="H16" s="1" t="str">
         <f t="shared" si="2"/>
         <v>C</v>
       </c>
@@ -1063,27 +1069,27 @@
       <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>75</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>72</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>87</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>53</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="G17" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>Pass</v>
-      </c>
-      <c r="H17" s="2" t="str">
+      <c r="G17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Pass</v>
+      </c>
+      <c r="H17" s="1" t="str">
         <f t="shared" si="2"/>
         <v>C</v>
       </c>
@@ -1092,27 +1098,27 @@
       <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>90</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>97</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>100</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <v>97</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
-      <c r="G18" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>Pass</v>
-      </c>
-      <c r="H18" s="2" t="str">
+      <c r="G18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Pass</v>
+      </c>
+      <c r="H18" s="1" t="str">
         <f t="shared" si="2"/>
         <v>A</v>
       </c>
@@ -1121,27 +1127,27 @@
       <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>95</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>80</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <v>88</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="1">
         <v>89</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
-      <c r="G19" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>Pass</v>
-      </c>
-      <c r="H19" s="2" t="str">
+      <c r="G19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Pass</v>
+      </c>
+      <c r="H19" s="1" t="str">
         <f t="shared" si="2"/>
         <v>B</v>
       </c>
@@ -1150,27 +1156,27 @@
       <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>66</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>100</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>93</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <v>82</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="G20" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>Pass</v>
-      </c>
-      <c r="H20" s="2" t="str">
+      <c r="G20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Pass</v>
+      </c>
+      <c r="H20" s="1" t="str">
         <f t="shared" si="2"/>
         <v>B</v>
       </c>
@@ -1179,27 +1185,27 @@
       <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>46</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>74</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>92</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="1">
         <v>87</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="1">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="G21" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>Pass</v>
-      </c>
-      <c r="H21" s="2" t="str">
+      <c r="G21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Pass</v>
+      </c>
+      <c r="H21" s="1" t="str">
         <f t="shared" si="2"/>
         <v>C</v>
       </c>
@@ -1208,27 +1214,27 @@
       <c r="A22" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>94</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>92</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
         <v>86</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="1">
         <v>100</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="1">
         <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="G22" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>Pass</v>
-      </c>
-      <c r="H22" s="2" t="str">
+      <c r="G22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Pass</v>
+      </c>
+      <c r="H22" s="1" t="str">
         <f t="shared" si="2"/>
         <v>A</v>
       </c>
@@ -1237,27 +1243,27 @@
       <c r="A23" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>55</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>52</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>76</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="1">
         <v>48</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="1">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="G23" s="2" t="str">
+      <c r="G23" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Fail</v>
       </c>
-      <c r="H23" s="2" t="str">
+      <c r="H23" s="1" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -1266,27 +1272,27 @@
       <c r="A24" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>41</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>44</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <v>95</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="1">
         <v>55</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="G24" s="2" t="str">
+      <c r="G24" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Fail</v>
       </c>
-      <c r="H24" s="2" t="str">
+      <c r="H24" s="1" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
@@ -1295,27 +1301,27 @@
       <c r="A25" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>53</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>97</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <v>74</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="1">
         <v>53</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="1">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
-      <c r="G25" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>Pass</v>
-      </c>
-      <c r="H25" s="2" t="str">
+      <c r="G25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Pass</v>
+      </c>
+      <c r="H25" s="1" t="str">
         <f t="shared" si="2"/>
         <v>D</v>
       </c>
@@ -1336,96 +1342,96 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="134.5" style="3" customWidth="1"/>
+    <col min="1" max="1" width="134.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>